<commit_message>
MODIFY ENTRUST DATA IMPORT TEMPLATE [CITIC_N]
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/DataTemplate/Entrust/CITIC_N.xlsx
+++ b/src/Presentation/CTM.Win/DataTemplate/Entrust/CITIC_N.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubRepo\CTM\CTM.Win\DataImportTemplate\Entrust\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source\ncCTM\src\Presentation\CTM.Win\DataTemplate\Entrust\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>委托时间</t>
   </si>
@@ -51,9 +51,6 @@
     <t>成交价格</t>
   </si>
   <si>
-    <t>合同编号</t>
-  </si>
-  <si>
     <t>申请编号</t>
   </si>
   <si>
@@ -78,34 +75,30 @@
     <t>委托</t>
   </si>
   <si>
-    <t>易事特</t>
-  </si>
-  <si>
     <t>已成</t>
   </si>
   <si>
-    <t>贝因美</t>
-  </si>
-  <si>
-    <t>证券卖出</t>
-  </si>
-  <si>
-    <t>部撤</t>
+    <t>波段</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>股东代码</t>
+  </si>
+  <si>
+    <t>交易市场</t>
   </si>
   <si>
     <t>交易类别</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>日内</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>帝王洁具</t>
+  </si>
+  <si>
+    <t>深圳</t>
   </si>
   <si>
     <t>波段</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>目标</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1052,227 +1045,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>0.5743287037037037</v>
+      </c>
+      <c r="B2">
+        <v>2761</v>
+      </c>
+      <c r="C2">
+        <v>2798</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>37.479999999999997</v>
+      </c>
+      <c r="I2">
+        <v>500</v>
+      </c>
+      <c r="J2">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="K2">
+        <v>500</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>211848625</v>
+      </c>
+      <c r="N2">
+        <v>1018000349</v>
+      </c>
+      <c r="O2" t="s">
         <v>24</v>
       </c>
+      <c r="Q2">
+        <v>2761</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
-        <v>0.59056712962962965</v>
-      </c>
-      <c r="B2">
-        <v>2570</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>0.57446759259259261</v>
+      </c>
+      <c r="B3">
+        <v>2763</v>
+      </c>
+      <c r="C3">
+        <v>2798</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>37.479999999999997</v>
+      </c>
+      <c r="I3">
+        <v>800</v>
+      </c>
+      <c r="J3">
+        <v>37.463999999999999</v>
+      </c>
+      <c r="K3">
+        <v>800</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>211848625</v>
+      </c>
+      <c r="N3">
+        <v>1018000349</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3">
+        <v>2763</v>
+      </c>
+      <c r="R3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>10000</v>
-      </c>
-      <c r="G2">
-        <v>10000</v>
-      </c>
-      <c r="H2">
+      <c r="S3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>0.57550925925925933</v>
+      </c>
+      <c r="B4">
+        <v>2766</v>
+      </c>
+      <c r="C4">
+        <v>2798</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="I4">
+        <v>5700</v>
+      </c>
+      <c r="J4">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="K4">
+        <v>5700</v>
+      </c>
+      <c r="L4">
         <v>0</v>
       </c>
-      <c r="I2">
-        <v>12.66</v>
-      </c>
-      <c r="J2">
-        <v>12.66</v>
-      </c>
-      <c r="K2">
-        <v>4340</v>
-      </c>
-      <c r="L2">
-        <v>4340</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="M4">
+        <v>211848625</v>
+      </c>
+      <c r="N4">
+        <v>1018000349</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4">
+        <v>2766</v>
+      </c>
+      <c r="R4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>0.57571759259259259</v>
+      </c>
+      <c r="B5">
+        <v>2767</v>
+      </c>
+      <c r="C5">
+        <v>2798</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="N2">
-        <v>880000269825</v>
-      </c>
-      <c r="O2">
-        <v>4340</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="R2" t="s">
+      <c r="H5">
+        <v>37.6</v>
+      </c>
+      <c r="I5">
+        <v>20000</v>
+      </c>
+      <c r="J5">
+        <v>37.58</v>
+      </c>
+      <c r="K5">
+        <v>20000</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>211848625</v>
+      </c>
+      <c r="N5">
+        <v>1018000349</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5">
+        <v>2767</v>
+      </c>
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>0.5759953703703703</v>
+      </c>
+      <c r="B6">
+        <v>2769</v>
+      </c>
+      <c r="C6">
+        <v>2798</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>37.68</v>
+      </c>
+      <c r="I6">
+        <v>30000</v>
+      </c>
+      <c r="J6">
+        <v>37.68</v>
+      </c>
+      <c r="K6">
+        <v>30000</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>211848625</v>
+      </c>
+      <c r="N6">
+        <v>1018000349</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6">
+        <v>2769</v>
+      </c>
+      <c r="R6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>0.59729166666666667</v>
-      </c>
-      <c r="B3">
-        <v>300376</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>0.58422453703703703</v>
+      </c>
+      <c r="B7">
+        <v>3008</v>
+      </c>
+      <c r="C7">
+        <v>2798</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>37.68</v>
+      </c>
+      <c r="I7">
+        <v>20000</v>
+      </c>
+      <c r="J7">
+        <v>37.674999999999997</v>
+      </c>
+      <c r="K7">
+        <v>20000</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>211848625</v>
+      </c>
+      <c r="N7">
+        <v>1018000349</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7">
+        <v>3008</v>
+      </c>
+      <c r="R7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>0.60089120370370364</v>
+      </c>
+      <c r="B8">
+        <v>3081</v>
+      </c>
+      <c r="C8">
+        <v>2798</v>
+      </c>
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="F3">
-        <v>10000</v>
-      </c>
-      <c r="G3">
-        <v>6400</v>
-      </c>
-      <c r="H3">
-        <v>3600</v>
-      </c>
-      <c r="I3">
-        <v>26.89</v>
-      </c>
-      <c r="J3">
-        <v>26.89</v>
-      </c>
-      <c r="K3">
-        <v>4491</v>
-      </c>
-      <c r="L3">
-        <v>4491</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>3</v>
       </c>
-      <c r="N3">
-        <v>880000269825</v>
-      </c>
-      <c r="O3">
-        <v>4491</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="R3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>0.5982291666666667</v>
-      </c>
-      <c r="B4">
-        <v>300376</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>3600</v>
-      </c>
-      <c r="G4">
-        <v>3600</v>
-      </c>
-      <c r="H4">
+      <c r="H8">
+        <v>38.270000000000003</v>
+      </c>
+      <c r="I8">
+        <v>24300</v>
+      </c>
+      <c r="J8">
+        <v>38.222999999999999</v>
+      </c>
+      <c r="K8">
+        <v>24300</v>
+      </c>
+      <c r="L8">
         <v>0</v>
       </c>
-      <c r="I4">
-        <v>26.85</v>
-      </c>
-      <c r="J4">
-        <v>26.85</v>
-      </c>
-      <c r="K4">
-        <v>4518</v>
-      </c>
-      <c r="L4">
-        <v>4518</v>
-      </c>
-      <c r="M4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4">
-        <v>880000269825</v>
-      </c>
-      <c r="O4">
-        <v>4518</v>
-      </c>
-      <c r="P4" t="s">
-        <v>18</v>
-      </c>
-      <c r="R4" t="s">
-        <v>27</v>
+      <c r="M8">
+        <v>211848625</v>
+      </c>
+      <c r="N8">
+        <v>1018000349</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8">
+        <v>3081</v>
+      </c>
+      <c r="R8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>